<commit_message>
Update Results PS - Olaru
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{65210D10-1889-42B4-916B-DD658CC8FA45}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{BDED3584-674C-4B4D-BD08-FB836A177413}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel_Prob_Stat" sheetId="1" r:id="rId1"/>
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1972,15 +1972,15 @@
         <v>82</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>4.7809523809523817</v>
+        <v>6.1809523809523812</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Results Stat updated and PS and Biostat
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{BDED3584-674C-4B4D-BD08-FB836A177413}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{F998CD64-2000-4DDD-B157-E525C81D26A5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1491,15 +1491,15 @@
         <v>85</v>
       </c>
       <c r="I2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J2">
         <f>MAX(4, ROUND(MIN(10, 1+0.5*I2/5+0.2*H2/10+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6)),0))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L2">
         <f>MIN(10, 1+0.5*I2/5+0.2*H2/10+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
-        <v>8.432380952380953</v>
+        <v>8.5323809523809526</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Biostat and Stat Tools for Finance courses up
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat_c.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{F998CD64-2000-4DDD-B157-E525C81D26A5}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{44E12E54-3B45-4B7E-BE46-A36CEC7FD0CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{0374533B-1CAF-4F1A-AC3C-C3558E00BA22}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1422,10 +1422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1465,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>8.5323809523809526</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>7.1376190476190473</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>6.1071428571428577</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>3.3666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>5.1204761904761913</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>6.1428571428571432</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>1.7819047619047619</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>4.2752380952380955</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>4.8885714285714288</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>7.3595238095238091</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>7.7614285714285716</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>6.1809523809523812</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>4.6885714285714286</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>6.4014285714285712</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>5.4719047619047618</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>7.5038095238095242</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>6.0847619047619048</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2316,7 +2317,7 @@
         <v>4.5038095238095242</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>4.1542857142857148</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>3.1419047619047618</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2427,7 +2428,7 @@
         <v>5.8999999999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>5.4499999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>5.5647619047619052</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>2.2104761904761903</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>6.0399999999999991</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>1.5161904761904763</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>6.1047619047619044</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>5.6871428571428577</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>5.4057142857142857</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>3.1714285714285713</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2834,7 +2835,7 @@
         <v>5.1657142857142855</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>1.9157142857142857</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>6.9223809523809514</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>2.1890476190476189</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2982,7 +2983,7 @@
         <v>4.5066666666666659</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>2.0123809523809522</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>5.7428571428571429</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -3130,7 +3131,7 @@
         <v>6.3938095238095247</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>7.9509523809523808</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>2.0152380952380953</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>4.5085714285714289</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>7.0842857142857136</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -3315,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>6.9095238095238098</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3389,7 +3390,7 @@
         <v>7.8009523809523813</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>5.961904761904762</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>7.4171428571428581</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>2.5695238095238095</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -3648,7 +3649,7 @@
         <v>6.7009523809523799</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>6.5904761904761902</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -3722,7 +3723,7 @@
         <v>3.9314285714285715</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>6.7914285714285718</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -3796,7 +3797,7 @@
         <v>8.1066666666666656</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -3833,7 +3834,7 @@
         <v>5.2495238095238097</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>3.6257142857142854</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3907,7 +3908,7 @@
         <v>5.4923809523809517</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>7.7457142857142856</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -4018,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>5.293333333333333</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>5.6914285714285722</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -5313,7 +5314,7 @@
         <v>3.0900000000000003</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -5351,7 +5352,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="244"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="L1:L1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>4.05</formula>

</xml_diff>